<commit_message>
feat(store): added simple event storage
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1DA50C-F225-4F02-B3DE-0709375A5E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F524F2-C159-4E40-914E-CAF1AC01C36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>KW</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Bugfix starttime timestamp</t>
+  </si>
+  <si>
+    <t>Simples speichern von Terminen in CSV-Dateien</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +515,7 @@
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -716,7 +719,16 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45270</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -729,7 +741,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -742,7 +754,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>7.6</v>
+        <v>8</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>

</xml_diff>

<commit_message>
chore(store): trying to bugfix format
Need to evaluate vars, custom vars with let work properly / as expected
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F524F2-C159-4E40-914E-CAF1AC01C36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9E99AA-BD27-4433-ACB2-D0B17763B871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>KW</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Simples speichern von Terminen in CSV-Dateien</t>
+  </si>
+  <si>
+    <t>Bugfixing / Recherche format Probleme (Linewrapping)</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +540,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -734,14 +737,23 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45271</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
       <c r="K15" t="s">
         <v>4</v>
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -754,7 +766,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>8</v>
+        <v>8.6</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>

</xml_diff>

<commit_message>
feat: better storing + parsing
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4713696B-987E-42AD-8B48-6354C8CC567D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A119A-5C85-499C-8A0A-ECDDE2544DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="1500" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="1845" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>KW</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Simples Speichern von Terminen in CSV-Dateien</t>
+  </si>
+  <si>
+    <t>Überarbeiten des Parsens und Speicherns der Events</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +546,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -756,7 +759,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -778,104 +781,113 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>9.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45274</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>52</v>

</xml_diff>

<commit_message>
feat(show): better display of multi day events
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A119A-5C85-499C-8A0A-ECDDE2544DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE53D6F-E3D0-41BC-85A9-122A4DEDB040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1845" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>KW</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Überarbeiten des Parsens und Speicherns der Events</t>
+  </si>
+  <si>
+    <t>Verbessern der Lesbarkeit beim Anzeigen von (mehrtägigen) Events</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -759,7 +762,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -781,11 +784,11 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>10</v>
+        <v>7.7</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,7 +809,16 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45275</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(store): merge sort database
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBF9CF5-95C4-43D5-AF46-504D7D901192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692119BC-3AC7-4F37-8F80-C930A3473C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8655" yWindow="3135" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>KW</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Umstrukturierung der Dateien, Entfernen alter Events</t>
+  </si>
+  <si>
+    <t>Implementierung MergeSort der Datenbank</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +555,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -765,7 +768,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
@@ -842,7 +845,16 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45275</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(import): multi event import from single file
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692119BC-3AC7-4F37-8F80-C930A3473C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6ABF59-AE31-416E-B845-050C0A75F68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>KW</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Implementierung MergeSort der Datenbank</t>
+  </si>
+  <si>
+    <t>Importieren mehrerer Events aus einer ICS-Datei</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -768,7 +771,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>34</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -790,7 +793,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
@@ -860,7 +863,16 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45276</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(delete): return empty file
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6ABF59-AE31-416E-B845-050C0A75F68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C2419F-D0DC-4685-9129-D6631491DA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>KW</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Importieren mehrerer Events aus einer ICS-Datei</t>
+  </si>
+  <si>
+    <t>Implementierung delete-command (leeren der Datenbank)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +583,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -771,7 +774,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>34.5</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -793,7 +796,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
@@ -878,7 +881,16 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45279</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(import): remove LF and CR
</commit_message>
<xml_diff>
--- a/docs/timesheet/timesheet.xlsx
+++ b/docs/timesheet/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\Ubuntu2004\shared\lisp-ical-cli\docs\timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36D434D-F05D-43CB-A812-2144A67C0460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B98C9B8-D045-4697-947C-82063749C973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>KW</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Implementierung inspect command (iterating through events)</t>
+  </si>
+  <si>
+    <t>Implementierung inspect command + besseres Display summary/description</t>
+  </si>
+  <si>
+    <t>Bugfix remove Linefeed + Carriage Return</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +595,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -780,7 +786,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>39.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -802,7 +808,7 @@
       </c>
       <c r="L16">
         <f ca="1">ROUNDDOWN(L15/M16,1)</f>
-        <v>7.9</v>
+        <v>8.5</v>
       </c>
       <c r="M16">
         <f ca="1">ROUNDDOWN((DATEDIF($B$2,TODAY(),"d")/7)+1,0)</f>
@@ -932,13 +938,31 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45283</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45284</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>